<commit_message>
Update guia de permutación y correlación
</commit_message>
<xml_diff>
--- a/Clase_05/Royal.xlsx
+++ b/Clase_05/Royal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Dropbox/CURSOS/PREGRADO/NUEVOS/OCE_313_TECNICAS_ANALISIS_NO_PARAMETRICOS/2022/MetodosNoParametricosv22/Clase_05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86C8277-B2F9-4E4B-9583-F2727273DC91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60834FD-9566-BA4C-B305-2F93658E8DFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" xr2:uid="{4274DD6F-DEFC-C841-B26F-67B1519BFDA9}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" activeTab="1" xr2:uid="{4274DD6F-DEFC-C841-B26F-67B1519BFDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0197CBE3-4734-5A44-B3E5-676D2CA08872}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -671,9 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA6F943-7BD5-5449-9276-C421644FB5D9}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>